<commit_message>
Random Forest algoritması için Final model eğitimi tamamlandı.
</commit_message>
<xml_diff>
--- a/notes/Anxiety-Model-Versus.xlsx
+++ b/notes/Anxiety-Model-Versus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code\Anxiety-Analysis-ML\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8E7252-B5F9-46CA-80A9-AF1F74DBAC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4BDFDB-2BEA-43F8-8F6F-4C918CE9DF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -153,49 +153,52 @@
     <t>MODEL:</t>
   </si>
   <si>
-    <t>0.8923</t>
-  </si>
-  <si>
-    <t>0.8929</t>
-  </si>
-  <si>
-    <t>0.9542</t>
-  </si>
-  <si>
-    <t>anxiety_model_20250510_0215</t>
-  </si>
-  <si>
-    <t>→Anksiyete (83.78%)</t>
-  </si>
-  <si>
-    <t>→Normal (15.61%)</t>
-  </si>
-  <si>
-    <t>→Anksiyete (66.74%)</t>
-  </si>
-  <si>
-    <t>→Normal (5.69%)</t>
-  </si>
-  <si>
-    <t>→Normal (29.68%)</t>
-  </si>
-  <si>
-    <t>→Normal (24.57%)</t>
-  </si>
-  <si>
-    <t>→Normal (40.25%)</t>
-  </si>
-  <si>
-    <t>→Normal (7.87%)</t>
-  </si>
-  <si>
-    <t>→Normal (38.18%)</t>
-  </si>
-  <si>
-    <t>→Normal (5.84%)</t>
-  </si>
-  <si>
     <t>Random Forest</t>
+  </si>
+  <si>
+    <t>0.8926</t>
+  </si>
+  <si>
+    <t>0.8958</t>
+  </si>
+  <si>
+    <t>0.8952</t>
+  </si>
+  <si>
+    <t>0.9550</t>
+  </si>
+  <si>
+    <t>anxiety_model_20250510_1009</t>
+  </si>
+  <si>
+    <t>→Anksiyete (84.31%)</t>
+  </si>
+  <si>
+    <t>→Normal (14.91%)</t>
+  </si>
+  <si>
+    <t>→Anksiyete (69.31%)</t>
+  </si>
+  <si>
+    <t>→Normal (5.23%)</t>
+  </si>
+  <si>
+    <t>→Normal (30.06%)</t>
+  </si>
+  <si>
+    <t>→Normal (24.60%)</t>
+  </si>
+  <si>
+    <t>→Normal (41.52%)</t>
+  </si>
+  <si>
+    <t>→Normal (8.27%)</t>
+  </si>
+  <si>
+    <t>→Normal (38.21%)</t>
+  </si>
+  <si>
+    <t>→Normal (5.13%)</t>
   </si>
 </sst>
 </file>
@@ -631,7 +634,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -664,7 +667,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -694,7 +697,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -724,7 +727,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -754,7 +757,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -784,7 +787,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -814,7 +817,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -844,7 +847,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -874,7 +877,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -904,7 +907,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -934,7 +937,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -964,7 +967,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -990,7 +993,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>22</v>
@@ -1010,7 +1013,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>23</v>
@@ -1030,7 +1033,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>24</v>
@@ -1050,7 +1053,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
SVM algoritması için Linear ve RBF biçiminde modeller eğitildi ve sonuçlar kaydedildi.
</commit_message>
<xml_diff>
--- a/notes/Anxiety-Model-Versus.xlsx
+++ b/notes/Anxiety-Model-Versus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code\Anxiety-Analysis-ML\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4BDFDB-2BEA-43F8-8F6F-4C918CE9DF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B514D2-32CF-4325-AC6F-24733C111725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -114,9 +114,6 @@
     <t>ROC AUC SCORE:</t>
   </si>
   <si>
-    <t xml:space="preserve">CROSS VALIDATION  ACCURACY: </t>
-  </si>
-  <si>
     <t>Metin 1-</t>
   </si>
   <si>
@@ -171,34 +168,133 @@
     <t>anxiety_model_20250510_1009</t>
   </si>
   <si>
-    <t>→Anksiyete (84.31%)</t>
-  </si>
-  <si>
-    <t>→Normal (14.91%)</t>
-  </si>
-  <si>
-    <t>→Anksiyete (69.31%)</t>
-  </si>
-  <si>
-    <t>→Normal (5.23%)</t>
-  </si>
-  <si>
-    <t>→Normal (30.06%)</t>
-  </si>
-  <si>
-    <t>→Normal (24.60%)</t>
-  </si>
-  <si>
-    <t>→Normal (41.52%)</t>
-  </si>
-  <si>
-    <t>→Normal (8.27%)</t>
-  </si>
-  <si>
-    <t>→Normal (38.21%)</t>
-  </si>
-  <si>
-    <t>→Normal (5.13%)</t>
+    <t>Anksiyete (84.31%)</t>
+  </si>
+  <si>
+    <t>Normal (14.91%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (69.31%)</t>
+  </si>
+  <si>
+    <t>Normal (5.23%)</t>
+  </si>
+  <si>
+    <t>Normal (30.06%)</t>
+  </si>
+  <si>
+    <t>Normal (24.60%)</t>
+  </si>
+  <si>
+    <t>Normal (41.52%)</t>
+  </si>
+  <si>
+    <t>Normal (8.27%)</t>
+  </si>
+  <si>
+    <t>Normal (38.21%)</t>
+  </si>
+  <si>
+    <t>Normal (5.13%)</t>
+  </si>
+  <si>
+    <t>0.9202</t>
+  </si>
+  <si>
+    <t>0.9254</t>
+  </si>
+  <si>
+    <t>0.9239</t>
+  </si>
+  <si>
+    <t>0.9749</t>
+  </si>
+  <si>
+    <t>RBF SVM</t>
+  </si>
+  <si>
+    <t>anxiety_model_20250510_1519</t>
+  </si>
+  <si>
+    <t>Anksiyete (75.17%)</t>
+  </si>
+  <si>
+    <t>Normal (38.30%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (78.01%)</t>
+  </si>
+  <si>
+    <t>Normal (26.02%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (55.40%)</t>
+  </si>
+  <si>
+    <t>Normal (48.54%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (59.60%)</t>
+  </si>
+  <si>
+    <t>Normal (35.28%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (54.88%)</t>
+  </si>
+  <si>
+    <t>Normal (25.22%)</t>
+  </si>
+  <si>
+    <t>CROSS VALIDATION  ACCURACY:</t>
+  </si>
+  <si>
+    <t>Linear SVM</t>
+  </si>
+  <si>
+    <t>0.9188</t>
+  </si>
+  <si>
+    <t>0.9251</t>
+  </si>
+  <si>
+    <t>0.9241</t>
+  </si>
+  <si>
+    <t>0.9742</t>
+  </si>
+  <si>
+    <t>anxiety_model_20250510_1849</t>
+  </si>
+  <si>
+    <t>Anksiyete (80.24%)</t>
+  </si>
+  <si>
+    <t>Normal (33.03%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (85.16%)</t>
+  </si>
+  <si>
+    <t>Normal (18.81%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (58.30%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (55.79%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (67.67%)</t>
+  </si>
+  <si>
+    <t>Normal (36.99%)</t>
+  </si>
+  <si>
+    <t>Anksiyete (52.81%)</t>
+  </si>
+  <si>
+    <t>Normal (17.71%)</t>
   </si>
 </sst>
 </file>
@@ -634,50 +730,58 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
     <col min="2" max="8" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -685,8 +789,12 @@
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -697,17 +805,21 @@
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>2</v>
@@ -715,8 +827,12 @@
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -727,17 +843,21 @@
         <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+        <v>48</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>3</v>
@@ -745,8 +865,12 @@
       <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -757,17 +881,21 @@
         <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>4</v>
@@ -775,8 +903,12 @@
       <c r="C9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -787,17 +919,21 @@
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
@@ -805,8 +941,12 @@
       <c r="C11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -817,17 +957,21 @@
         <v>15</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>6</v>
@@ -835,8 +979,12 @@
       <c r="C13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -847,17 +995,21 @@
         <v>16</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+        <v>52</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>7</v>
@@ -865,8 +1017,12 @@
       <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -877,17 +1033,21 @@
         <v>17</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>8</v>
@@ -895,8 +1055,12 @@
       <c r="C17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -907,17 +1071,21 @@
         <v>18</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+        <v>54</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>9</v>
@@ -925,8 +1093,12 @@
       <c r="C19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -937,17 +1109,21 @@
         <v>19</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>10</v>
@@ -955,8 +1131,12 @@
       <c r="C21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -967,10 +1147,14 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+        <v>56</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -987,19 +1171,19 @@
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -1013,13 +1197,13 @@
         <v>23</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -1033,13 +1217,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -1053,13 +1237,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>

</xml_diff>

<commit_message>
Multinomial Naive Bayes modeli de eğitildi ve eğitimlerin sonuna gelindi.
</commit_message>
<xml_diff>
--- a/notes/Anxiety-Model-Versus.xlsx
+++ b/notes/Anxiety-Model-Versus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code\Anxiety-Analysis-ML\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B514D2-32CF-4325-AC6F-24733C111725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A98C379-7795-467F-B6CC-43D27773881A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="106">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -295,6 +295,54 @@
   </si>
   <si>
     <t>Normal (17.71%)</t>
+  </si>
+  <si>
+    <t>Multinomial Naive Bayes</t>
+  </si>
+  <si>
+    <t>0.8992</t>
+  </si>
+  <si>
+    <t>0.8972</t>
+  </si>
+  <si>
+    <t>0.9018</t>
+  </si>
+  <si>
+    <t>0.9708</t>
+  </si>
+  <si>
+    <t>anxiety_model_20250510_2039</t>
+  </si>
+  <si>
+    <t>→Anksiyete (98.64%)</t>
+  </si>
+  <si>
+    <t>→Anksiyete (59.12%)</t>
+  </si>
+  <si>
+    <t>→Anksiyete (98.38%)</t>
+  </si>
+  <si>
+    <t>→Normal (18.99%)</t>
+  </si>
+  <si>
+    <t>→Anksiyete (87.41%)</t>
+  </si>
+  <si>
+    <t>→Anksiyete (83.68%)</t>
+  </si>
+  <si>
+    <t>→Anksiyete (94.38%)</t>
+  </si>
+  <si>
+    <t>→Anksiyete (64.69%)</t>
+  </si>
+  <si>
+    <t>→Anksiyete (96.03%)</t>
+  </si>
+  <si>
+    <t>→Normal (47.84%)</t>
   </si>
 </sst>
 </file>
@@ -729,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,7 +803,9 @@
       <c r="E1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
@@ -775,7 +825,9 @@
       <c r="E2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
@@ -795,7 +847,9 @@
       <c r="E3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
@@ -813,7 +867,9 @@
       <c r="E4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>96</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
@@ -833,7 +889,9 @@
       <c r="E5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
@@ -851,7 +909,9 @@
       <c r="E6" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -871,7 +931,9 @@
       <c r="E7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
@@ -889,7 +951,9 @@
       <c r="E8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
@@ -909,7 +973,9 @@
       <c r="E9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
@@ -927,7 +993,9 @@
       <c r="E10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
@@ -947,7 +1015,9 @@
       <c r="E11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
@@ -965,7 +1035,9 @@
       <c r="E12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
@@ -985,7 +1057,9 @@
       <c r="E13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
@@ -1003,7 +1077,9 @@
       <c r="E14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
@@ -1023,7 +1099,9 @@
       <c r="E15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
@@ -1041,7 +1119,9 @@
       <c r="E16" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
@@ -1061,7 +1141,9 @@
       <c r="E17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
@@ -1079,7 +1161,9 @@
       <c r="E18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
@@ -1099,7 +1183,9 @@
       <c r="E19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
@@ -1117,7 +1203,9 @@
       <c r="E20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
@@ -1137,7 +1225,9 @@
       <c r="E21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
@@ -1155,7 +1245,9 @@
       <c r="E22" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
@@ -1185,7 +1277,9 @@
       <c r="E24" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
     </row>
@@ -1205,7 +1299,9 @@
       <c r="E25" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="10"/>
+      <c r="F25" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
@@ -1225,7 +1321,9 @@
       <c r="E26" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
@@ -1245,7 +1343,9 @@
       <c r="E27" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="10"/>
+      <c r="F27" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
     </row>

</xml_diff>